<commit_message>
Updated modules and enabled concurrent server-client run
Updated several project modules and updated project setup to run server and client concurrently using concurrently package.
</commit_message>
<xml_diff>
--- a/Life/server/data/lifelink_db.xlsx
+++ b/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -708,16 +708,54 @@
         <v>45952.68241876157</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>691738fd297efcf2c86dd197</v>
+      </c>
+      <c r="B10" t="str">
+        <v>xyz</v>
+      </c>
+      <c r="C10" t="str">
+        <v>xyz@gmail.com</v>
+      </c>
+      <c r="D10" t="str">
+        <v>9538825393</v>
+      </c>
+      <c r="E10" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F10" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>45975.8218484838</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -942,13 +980,45 @@
       <c r="I7" t="str">
         <v>Low</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7">
         <v>45952.68241974537</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>6917500ffc104a03933292da</v>
+      </c>
+      <c r="B8" t="str">
+        <v>abc</v>
+      </c>
+      <c r="C8" t="str">
+        <v>abc@gmail.com</v>
+      </c>
+      <c r="D8" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="E8" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F8" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="str">
+        <v>High</v>
+      </c>
+      <c r="J8" s="1">
+        <v>45975.89019929398</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove large node_modules files
</commit_message>
<xml_diff>
--- a/Life/server/data/lifelink_db.xlsx
+++ b/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -780,13 +780,127 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11">
         <v>45984.95185159722</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>69234632a9d7b28957d0eb0c</v>
+      </c>
+      <c r="B12" t="str">
+        <v>mno</v>
+      </c>
+      <c r="C12" t="str">
+        <v>mno@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>9481824919</v>
+      </c>
+      <c r="E12" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>45984.96320155093</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>69234680a9d7b28957d0eb11</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Me</v>
+      </c>
+      <c r="C13" t="str">
+        <v>23a43.bhavish@sjec.ac.in</v>
+      </c>
+      <c r="D13" t="str">
+        <v>8904534919</v>
+      </c>
+      <c r="E13" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>45984.9641012037</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>6923b7181c52f11af60577df</v>
+      </c>
+      <c r="B14" t="str">
+        <v>mailtrap</v>
+      </c>
+      <c r="C14" t="str">
+        <v>lifelink@system.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>1234456789</v>
+      </c>
+      <c r="E14" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1">
+        <v>45985.297717719906</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L14"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
updated code of the project
</commit_message>
<xml_diff>
--- a/Life/server/data/lifelink_db.xlsx
+++ b/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -936,9 +936,47 @@
         <v>45989.81751922454</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>692a4edc07042cb8aa370cd8</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C16" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E16" t="str">
+        <v>O+</v>
+      </c>
+      <c r="F16" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G16">
+        <v>75.1239547</v>
+      </c>
+      <c r="H16">
+        <v>15.3647083</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16" s="1">
+        <v>45990.29850224537</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L16"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1266,7 +1304,7 @@
       <c r="I10" t="str">
         <v>Critical</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10">
         <v>45989.91622431713</v>
       </c>
     </row>

</xml_diff>